<commit_message>
Lernjournal angepasst und Aktivitätsdiagram begonnen
</commit_message>
<xml_diff>
--- a/aufgabe_1+2_team_3.xlsx
+++ b/aufgabe_1+2_team_3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -107,6 +107,9 @@
   <si>
     <t>Erweitern des Dokumentes und erstellen der Struktur(en)
 Erstellen eines Branches für die "alte" Aufgabe (Aufgabe_1). Weiterarbeit auf "master".</t>
+  </si>
+  <si>
+    <t>Andwenungsfalldiagramm erstellt</t>
   </si>
 </sst>
 </file>
@@ -669,7 +672,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1130,9 +1133,15 @@
       <c r="P23" s="10"/>
     </row>
     <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="8">
+        <v>75</v>
+      </c>
+      <c r="C24" s="9">
+        <v>41385</v>
+      </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -1243,7 +1252,7 @@
       </c>
       <c r="B30" s="18">
         <f>SUM(B23:B29)</f>
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="2"/>
@@ -1473,11 +1482,11 @@
       </c>
       <c r="B42" s="16">
         <f>SUM(B30,B16)</f>
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="C42" s="17">
         <f>TIME(0,B42,)</f>
-        <v>2.7777777777777776E-2</v>
+        <v>7.9861111111111119E-2</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>

</xml_diff>

<commit_message>
Zusammnarbeit am Dokument (Prorisierung, UC Diagram, etc), gitignor angepasst und Word version geUpdated
</commit_message>
<xml_diff>
--- a/aufgabe_1+2_team_3.xlsx
+++ b/aufgabe_1+2_team_3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -109,7 +109,11 @@
 Erstellen eines Branches für die "alte" Aufgabe (Aufgabe_1). Weiterarbeit auf "master".</t>
   </si>
   <si>
-    <t>Andwenungsfalldiagramm erstellt</t>
+    <t>Aufgaben verteilt (Anwendungsfälle beschreiben), Priorisierung, Anwendungsfalldiagramm besprochen.
+Grundlegend Organisation der Arbeiten an der Aufgabe 2</t>
+  </si>
+  <si>
+    <t>Andwenungsfalldiagramm erstellt, Anwendugsfälle "bestimmt".</t>
   </si>
 </sst>
 </file>
@@ -228,8 +232,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -315,7 +321,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -328,6 +334,7 @@
     <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -340,6 +347,7 @@
     <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -672,7 +680,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -878,9 +886,15 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="8">
+        <v>120</v>
+      </c>
+      <c r="C11" s="9">
+        <v>41385</v>
+      </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -973,7 +987,7 @@
       </c>
       <c r="B16" s="18">
         <f>SUM(B11:B15)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
@@ -1134,7 +1148,7 @@
     </row>
     <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" s="8">
         <v>75</v>
@@ -1157,9 +1171,15 @@
       <c r="P24" s="10"/>
     </row>
     <row r="25" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
+      <c r="A25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="8">
+        <v>120</v>
+      </c>
+      <c r="C25" s="9">
+        <v>41385</v>
+      </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -1252,7 +1272,7 @@
       </c>
       <c r="B30" s="18">
         <f>SUM(B23:B29)</f>
-        <v>115</v>
+        <v>235</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="2"/>
@@ -1482,11 +1502,11 @@
       </c>
       <c r="B42" s="16">
         <f>SUM(B30,B16)</f>
-        <v>115</v>
+        <v>355</v>
       </c>
       <c r="C42" s="17">
         <f>TIME(0,B42,)</f>
-        <v>7.9861111111111119E-2</v>
+        <v>0.24652777777777779</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>

</xml_diff>

<commit_message>
Anwendungsfall "Kunde Erstellen" beschrieben und Aktivitätsdiagramm erstellt
</commit_message>
<xml_diff>
--- a/aufgabe_1+2_team_3.xlsx
+++ b/aufgabe_1+2_team_3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Andwenungsfalldiagramm erstellt, Anwendugsfälle "bestimmt".</t>
+  </si>
+  <si>
+    <t>Anwendungsfall "Kunde erstellen" beschreiben und Aktivitätsdiagram v0.1 gezeichnet.</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -318,6 +321,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="27">
@@ -679,7 +685,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -988,7 +994,10 @@
         <f>SUM(B11:B15)</f>
         <v>120</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="20">
+        <f>TIME(0,B16,)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1194,9 +1203,15 @@
       <c r="P25" s="10"/>
     </row>
     <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="8">
+        <v>65</v>
+      </c>
+      <c r="C26" s="9">
+        <v>41385</v>
+      </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -1271,9 +1286,12 @@
       </c>
       <c r="B30" s="18">
         <f>SUM(B23:B29)</f>
-        <v>235</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>300</v>
+      </c>
+      <c r="C30" s="20">
+        <f>TIME(0,B30,)</f>
+        <v>0.20833333333333334</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1472,7 +1490,7 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="1:16" s="4" customFormat="1">
+    <row r="40" spans="1:16" s="4" customFormat="1" hidden="1">
       <c r="A40" s="13" t="s">
         <v>8</v>
       </c>
@@ -1501,11 +1519,11 @@
       </c>
       <c r="B42" s="16">
         <f>SUM(B30,B16)</f>
-        <v>355</v>
+        <v>420</v>
       </c>
       <c r="C42" s="17">
         <f>TIME(0,B42,)</f>
-        <v>0.24652777777777779</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>

</xml_diff>

<commit_message>
Zusammenführen der Arbeiten, Tabelle Iterativ, Besprechung und  Lernjournal
</commit_message>
<xml_diff>
--- a/aufgabe_1+2_team_3.xlsx
+++ b/aufgabe_1+2_team_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="263"/>
+    <workbookView xWindow="1240" yWindow="0" windowWidth="23980" windowHeight="17020" tabRatio="350"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 2" sheetId="2" r:id="rId1"/>
     <sheet name="Lernjournal Aufgabe 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -105,10 +105,6 @@
     <t>Projektaufgabe (Titel): Anforderungsanalyse Aufgabe 2</t>
   </si>
   <si>
-    <t>Erweitern des Dokumentes und erstellen der Struktur(en)
-Erstellen eines Branches für die "alte" Aufgabe (Aufgabe_1). Weiterarbeit auf "master".</t>
-  </si>
-  <si>
     <t>Aufgaben verteilt (Anwendungsfälle beschreiben), Priorisierung, Anwendungsfalldiagramm besprochen.
 Grundlegend Organisation der Arbeiten an der Aufgabe 2</t>
   </si>
@@ -120,17 +116,29 @@
   </si>
   <si>
     <t>Anwendungsfall mit hoher Prio "Kunde löschen" und "Kunde suchen" beschrieben  Vorschlag für Iterationen (Teilaufgabe 6), nachforschen</t>
+  </si>
+  <si>
+    <t>Anwendungsfall Beschreibungen zusammegeführt
+Erarbeitung der Tabelle zum Iterativen Entwicklungsprozess
+Besprechung der Arbeit</t>
+  </si>
+  <si>
+    <t>Dokument vertigstellen (Lyout, Inhalte gestalten)</t>
+  </si>
+  <si>
+    <t>Erweitern des Dokumentes (Lyouten, erstellen der Struktur(en))
+Erstellen eines Branches für die "alte" Aufgabe (Aufgabe_1). Weiterarbeit auf "master".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="???\ &quot;Minuten&quot;"/>
     <numFmt numFmtId="165" formatCode="[hh]:mm\ &quot;Std:Min&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -166,6 +174,11 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,7 +250,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -265,8 +278,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -331,34 +348,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+  <cellStyles count="31">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -687,20 +723,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +812,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -832,7 +868,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -872,7 +908,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="10" spans="1:16" s="4" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -898,12 +934,12 @@
     </row>
     <row r="11" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="8">
+        <v>20</v>
+      </c>
+      <c r="B11" s="22">
         <v>120</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="23">
         <v>41385</v>
       </c>
       <c r="D11" s="10"/>
@@ -922,12 +958,12 @@
     </row>
     <row r="12" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
       <c r="A12" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="8">
+        <v>23</v>
+      </c>
+      <c r="B12" s="22">
         <v>90</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="23">
         <v>41385</v>
       </c>
       <c r="D12" s="10"/>
@@ -944,10 +980,16 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="22">
+        <v>105</v>
+      </c>
+      <c r="C13" s="23">
+        <v>41388</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1004,11 +1046,11 @@
       </c>
       <c r="B16" s="18">
         <f>SUM(B11:B15)</f>
-        <v>210</v>
+        <v>315</v>
       </c>
       <c r="C16" s="19">
         <f>TIME(0,B16,)</f>
-        <v>0.14583333333333334</v>
+        <v>0.21875</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1078,7 +1120,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="20" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
@@ -1118,7 +1160,7 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="22" spans="1:16" s="4" customFormat="1">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -1143,13 +1185,13 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="8">
+      <c r="A23" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="25">
         <v>40</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="26">
         <v>41384</v>
       </c>
       <c r="D23" s="10"/>
@@ -1166,14 +1208,14 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+    <row r="24" spans="1:16" s="11" customFormat="1">
       <c r="A24" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="8">
+        <v>21</v>
+      </c>
+      <c r="B24" s="22">
         <v>75</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="23">
         <v>41385</v>
       </c>
       <c r="D24" s="10"/>
@@ -1192,12 +1234,12 @@
     </row>
     <row r="25" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="8">
+        <v>20</v>
+      </c>
+      <c r="B25" s="22">
         <v>120</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="23">
         <v>41385</v>
       </c>
       <c r="D25" s="10"/>
@@ -1214,14 +1256,14 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+    <row r="26" spans="1:16" s="11" customFormat="1">
       <c r="A26" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="8">
+        <v>22</v>
+      </c>
+      <c r="B26" s="22">
         <v>65</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="23">
         <v>41385</v>
       </c>
       <c r="D26" s="10"/>
@@ -1238,10 +1280,16 @@
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
+    <row r="27" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="22">
+        <v>105</v>
+      </c>
+      <c r="C27" s="23">
+        <v>41388</v>
+      </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -1257,9 +1305,15 @@
       <c r="P27" s="10"/>
     </row>
     <row r="28" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
+      <c r="A28" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="25">
+        <v>30</v>
+      </c>
+      <c r="C28" s="26">
+        <v>41389</v>
+      </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -1298,11 +1352,11 @@
       </c>
       <c r="B30" s="18">
         <f>SUM(B23:B29)</f>
-        <v>300</v>
+        <v>435</v>
       </c>
       <c r="C30" s="19">
         <f>TIME(0,B30,)</f>
-        <v>0.20833333333333334</v>
+        <v>0.30208333333333331</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1372,7 +1426,7 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
+    <row r="34" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
       <c r="A34" s="5" t="s">
         <v>2</v>
       </c>
@@ -1412,7 +1466,7 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
+    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
       <c r="A36" s="6" t="s">
         <v>4</v>
       </c>
@@ -1525,17 +1579,17 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
       <c r="A42" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B42" s="16">
         <f>SUM(B30,B16)</f>
-        <v>510</v>
+        <v>750</v>
       </c>
       <c r="C42" s="17">
         <f>TIME(0,B42,)</f>
-        <v>0.35416666666666669</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1573,20 +1627,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1662,7 +1716,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -1718,7 +1772,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1758,7 +1812,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="10" spans="1:16" s="4" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1973,7 +2027,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="20" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
@@ -2013,7 +2067,7 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="22" spans="1:16" s="4" customFormat="1">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -2276,7 +2330,7 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
+    <row r="34" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
       <c r="A34" s="5" t="s">
         <v>2</v>
       </c>
@@ -2316,7 +2370,7 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
+    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
       <c r="A36" s="6" t="s">
         <v>4</v>
       </c>
@@ -2429,7 +2483,7 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
       <c r="A42" s="15" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Auftrag 6 angepasst, Endbesprechung und Lernjournal ergänzt
</commit_message>
<xml_diff>
--- a/aufgabe_1+2_team_3.xlsx
+++ b/aufgabe_1+2_team_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="350"/>
+    <workbookView xWindow="1240" yWindow="0" windowWidth="26660" windowHeight="18660" tabRatio="350"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 2" sheetId="2" r:id="rId1"/>
     <sheet name="Lernjournal Aufgabe 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -132,16 +132,19 @@
   <si>
     <t>Dokument durchgehen/überprüfen</t>
   </si>
+  <si>
+    <t>Abschlussbesprechung und Korrektur/Ergänzung des Auftrages 6 (Iteartionen)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="???\ &quot;Minuten&quot;"/>
     <numFmt numFmtId="165" formatCode="[hh]:mm\ &quot;Std:Min&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -253,8 +256,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -367,37 +372,39 @@
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+  <cellStyles count="33">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -726,20 +733,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E19" sqref="E18:E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +822,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -871,7 +878,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -911,7 +918,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="10" spans="1:16" s="4" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -983,7 +990,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="38.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="36">
       <c r="A13" s="8" t="s">
         <v>24</v>
       </c>
@@ -1007,7 +1014,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+    <row r="14" spans="1:16" s="11" customFormat="1">
       <c r="A14" s="20" t="s">
         <v>27</v>
       </c>
@@ -1031,10 +1038,16 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="12"/>
+    <row r="15" spans="1:16" s="11" customFormat="1">
+      <c r="A15" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8">
+        <v>45</v>
+      </c>
+      <c r="C15" s="9">
+        <v>41390</v>
+      </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1049,36 +1062,36 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" s="4" customFormat="1">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" s="4" customFormat="1">
+      <c r="A17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="18">
-        <f>SUM(B11:B15)</f>
-        <v>330</v>
-      </c>
-      <c r="C16" s="19">
-        <f>TIME(0,B16,)</f>
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" s="4" customFormat="1">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
+      <c r="B17" s="18">
+        <f>SUM(B11:B16)</f>
+        <v>375</v>
+      </c>
+      <c r="C17" s="19">
+        <f>TIME(0,B17,)</f>
+        <v>0.26041666666666669</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1129,14 +1142,10 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" ht="15.75">
-      <c r="A20" s="5" t="s">
-        <v>9</v>
-      </c>
+    <row r="20" spans="1:16" s="4" customFormat="1">
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1151,10 +1160,14 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="1:16" s="4" customFormat="1">
-      <c r="A21" s="2"/>
+    <row r="21" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A21" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1169,16 +1182,10 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" ht="25.5">
-      <c r="A22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>6</v>
-      </c>
+    <row r="22" spans="1:16" s="4" customFormat="1">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1193,39 +1200,39 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:16" s="4" customFormat="1">
+      <c r="A23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A24" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B24" s="24">
         <v>40</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C24" s="25">
         <v>41384</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-    </row>
-    <row r="24" spans="1:16" s="11" customFormat="1">
-      <c r="A24" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="21">
-        <v>75</v>
-      </c>
-      <c r="C24" s="22">
-        <v>41385</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -1241,12 +1248,12 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+    <row r="25" spans="1:16" s="11" customFormat="1">
       <c r="A25" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B25" s="21">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="C25" s="22">
         <v>41385</v>
@@ -1265,12 +1272,12 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5">
+    <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" s="21">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="C26" s="22">
         <v>41385</v>
@@ -1289,15 +1296,15 @@
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="1:16" s="11" customFormat="1" ht="38.25">
+    <row r="27" spans="1:16" s="11" customFormat="1">
       <c r="A27" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="21">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="C27" s="22">
-        <v>41388</v>
+        <v>41385</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -1313,15 +1320,15 @@
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A28" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="24">
-        <v>30</v>
-      </c>
-      <c r="C28" s="25">
-        <v>41389</v>
+    <row r="28" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A28" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="21">
+        <v>105</v>
+      </c>
+      <c r="C28" s="22">
+        <v>41388</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -1337,10 +1344,16 @@
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="12"/>
+    <row r="29" spans="1:16" s="11" customFormat="1">
+      <c r="A29" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="24">
+        <v>30</v>
+      </c>
+      <c r="C29" s="25">
+        <v>41389</v>
+      </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1355,54 +1368,60 @@
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="1:16" s="4" customFormat="1">
-      <c r="A30" s="13" t="s">
+    <row r="30" spans="1:16" s="11" customFormat="1">
+      <c r="A30" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="24">
+        <v>45</v>
+      </c>
+      <c r="C30" s="25">
+        <v>41390</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" s="4" customFormat="1">
+      <c r="A32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="18">
-        <f>SUM(B23:B29)</f>
-        <v>435</v>
-      </c>
-      <c r="C30" s="19">
-        <f>TIME(0,B30,)</f>
-        <v>0.30208333333333331</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-    </row>
-    <row r="31" spans="1:16" s="4" customFormat="1">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
+      <c r="B32" s="18">
+        <f>SUM(B24:B31)</f>
+        <v>480</v>
+      </c>
+      <c r="C32" s="19">
+        <f>TIME(0,B32,)</f>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1417,7 +1436,7 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="1:16" s="4" customFormat="1" hidden="1">
+    <row r="33" spans="1:16" s="4" customFormat="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
@@ -1435,14 +1454,10 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
-      <c r="A34" s="5" t="s">
-        <v>2</v>
-      </c>
+    <row r="34" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C34" s="3"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1475,15 +1490,13 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
-      <c r="A36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>6</v>
+    <row r="36" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+      <c r="A36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1499,58 +1512,58 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A39" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B39" s="8">
         <v>0</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C39" s="9">
         <v>41275</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-    </row>
-    <row r="38" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A38" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="8">
-        <v>0</v>
-      </c>
-      <c r="C38" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-    </row>
-    <row r="39" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="12"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -1565,41 +1578,57 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A40" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="8">
+        <v>0</v>
+      </c>
+      <c r="C40" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A42" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="14">
-        <f>SUM(B37:B39)</f>
+      <c r="B42" s="14">
+        <f>SUM(B39:B41)</f>
         <v>0</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-    </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A42" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="16">
-        <f>SUM(B30,B16)</f>
-        <v>765</v>
-      </c>
-      <c r="C42" s="17">
-        <f>TIME(0,B42,)</f>
-        <v>0.53125</v>
-      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1613,6 +1642,32 @@
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
+    </row>
+    <row r="44" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+      <c r="A44" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="16">
+        <f>SUM(B32,B17)</f>
+        <v>855</v>
+      </c>
+      <c r="C44" s="17">
+        <f>TIME(0,B44,)</f>
+        <v>0.59375</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1636,20 +1691,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1780,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -1781,7 +1836,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1821,7 +1876,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="10" spans="1:16" s="4" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -2036,7 +2091,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="20" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
@@ -2076,7 +2131,7 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="22" spans="1:16" s="4" customFormat="1">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -2339,7 +2394,7 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
+    <row r="34" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
       <c r="A34" s="5" t="s">
         <v>2</v>
       </c>
@@ -2379,7 +2434,7 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
+    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
       <c r="A36" s="6" t="s">
         <v>4</v>
       </c>
@@ -2492,7 +2547,7 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
       <c r="A42" s="15" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Letzte mini Korrekturen, erstellen der Abgabeversionen 1x Gesamt und 1x nur Aufgabe 2, Lernjournal ergänzt und von Aufgabe 2 als pdf erstellt.
</commit_message>
<xml_diff>
--- a/aufgabe_1+2_team_3.xlsx
+++ b/aufgabe_1+2_team_3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Abschlussbesprechung und Korrektur/Ergänzung des Auftrages 6 (Iteartionen)</t>
+  </si>
+  <si>
+    <t>Finish der gemiensamen Korrekturen und Layout ausputzen/fehler beheben</t>
   </si>
 </sst>
 </file>
@@ -256,8 +259,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -372,7 +377,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="35">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -389,6 +394,7 @@
     <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -405,6 +411,7 @@
     <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1392,10 +1399,16 @@
       <c r="O30" s="10"/>
       <c r="P30" s="10"/>
     </row>
-    <row r="31" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="12"/>
+    <row r="31" spans="1:16" s="11" customFormat="1">
+      <c r="A31" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="24">
+        <v>25</v>
+      </c>
+      <c r="C31" s="25">
+        <v>41399</v>
+      </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -1410,36 +1423,36 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="1:16" s="4" customFormat="1">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" s="4" customFormat="1">
+      <c r="A33" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="18">
-        <f>SUM(B24:B31)</f>
-        <v>480</v>
-      </c>
-      <c r="C32" s="19">
-        <f>TIME(0,B32,)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-    </row>
-    <row r="33" spans="1:16" s="4" customFormat="1">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
+      <c r="B33" s="18">
+        <f>SUM(B24:B32)</f>
+        <v>505</v>
+      </c>
+      <c r="C33" s="19">
+        <f>TIME(0,B33,)</f>
+        <v>0.35069444444444442</v>
+      </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1454,7 +1467,7 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" hidden="1">
+    <row r="34" spans="1:16" s="4" customFormat="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
@@ -1490,14 +1503,10 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
-      <c r="A36" s="5" t="s">
-        <v>2</v>
-      </c>
+    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C36" s="3"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1512,10 +1521,14 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A37" s="2"/>
+    <row r="37" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+      <c r="A37" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1531,15 +1544,9 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A38" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -1554,29 +1561,29 @@
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
     </row>
-    <row r="39" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A39" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="8">
-        <v>0</v>
-      </c>
-      <c r="C39" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
+    <row r="39" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A39" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A40" s="8" t="s">
@@ -1602,10 +1609,16 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="12"/>
+    <row r="41" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A41" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="8">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9">
+        <v>41275</v>
+      </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -1620,54 +1633,72 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A42" s="13" t="s">
+    <row r="42" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A43" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="14">
-        <f>SUM(B39:B41)</f>
+      <c r="B43" s="14">
+        <f>SUM(B40:B42)</f>
         <v>0</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-    </row>
-    <row r="44" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
-      <c r="A44" s="15" t="s">
+      <c r="C43" s="3"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="45" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+      <c r="A45" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="16">
-        <f>SUM(B32,B17)</f>
-        <v>855</v>
-      </c>
-      <c r="C44" s="17">
-        <f>TIME(0,B44,)</f>
-        <v>0.59375</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
+      <c r="B45" s="16">
+        <f>SUM(B33,B17)</f>
+        <v>880</v>
+      </c>
+      <c r="C45" s="17">
+        <f>TIME(0,B45,)</f>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>